<commit_message>
Tests, and import lib has been replaced to the more wide pandas
</commit_message>
<xml_diff>
--- a/dev/tests/data/test-odf.xlsx
+++ b/dev/tests/data/test-odf.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="test" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -28,22 +28,34 @@
     <t xml:space="preserve">quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">weigth</t>
+    <t xml:space="preserve">weight</t>
   </si>
   <si>
     <t xml:space="preserve">price</t>
   </si>
   <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
     <t xml:space="preserve">user</t>
   </si>
   <si>
     <t xml:space="preserve">etewrt</t>
   </si>
   <si>
-    <t xml:space="preserve">seva</t>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u1</t>
   </si>
   <si>
     <t xml:space="preserve">cvbncv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u2</t>
   </si>
 </sst>
 </file>
@@ -139,13 +151,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.04"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -163,10 +182,13 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -178,12 +200,15 @@
         <v>11.11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>112</v>
@@ -195,7 +220,10 @@
         <v>34.12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>